<commit_message>
database gebouwd en connection string, nuget package toegevoegd
</commit_message>
<xml_diff>
--- a/Documentatie/KT2/ad.2.1_Genormaliseerde_databaseontwerp.xlsx
+++ b/Documentatie/KT2/ad.2.1_Genormaliseerde_databaseontwerp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
   <si>
     <t>UserId</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>ScheduleId</t>
-  </si>
-  <si>
-    <t>Expired</t>
-  </si>
-  <si>
     <t>AppointmentId</t>
   </si>
   <si>
@@ -52,12 +46,6 @@
     <t>•GradeRowIndex</t>
   </si>
   <si>
-    <t>•ScheduleId</t>
-  </si>
-  <si>
-    <t>•Expired</t>
-  </si>
-  <si>
     <t>•AppointmentId</t>
   </si>
   <si>
@@ -73,9 +61,6 @@
     <t>Users (R1)</t>
   </si>
   <si>
-    <t>StartDate</t>
-  </si>
-  <si>
     <t>SubjectRowIndex</t>
   </si>
   <si>
@@ -124,16 +109,10 @@
     <t>•TaskLabel</t>
   </si>
   <si>
-    <t>•StartDate</t>
-  </si>
-  <si>
     <t>Appointments (R4)</t>
   </si>
   <si>
     <t>Subjects (R3)</t>
-  </si>
-  <si>
-    <t>Schedules (R2)</t>
   </si>
   <si>
     <t>Tasks (R5)</t>
@@ -181,9 +160,6 @@
     <t>Bachmandiagram</t>
   </si>
   <si>
-    <t>Schedules</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -194,6 +170,12 @@
   </si>
   <si>
     <t>Appointments</t>
+  </si>
+  <si>
+    <t>Tasks (R2)</t>
+  </si>
+  <si>
+    <t>Grades (R5)</t>
   </si>
 </sst>
 </file>
@@ -233,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -256,11 +238,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,6 +274,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,39 +297,39 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>869156</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>17859</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>666753</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>59120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>952501</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>125015</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="45" name="Group 44"/>
+        <xdr:cNvPr id="2" name="Group 1"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="869156" y="13733859"/>
-          <a:ext cx="1096075" cy="2030015"/>
-          <a:chOff x="869156" y="14495859"/>
-          <a:chExt cx="1095375" cy="2030015"/>
+          <a:off x="2560547" y="13203620"/>
+          <a:ext cx="285748" cy="1208895"/>
+          <a:chOff x="2565184" y="14537120"/>
+          <a:chExt cx="285748" cy="1208895"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="31" name="Elbow Connector 30"/>
+          <xdr:cNvPr id="38" name="Elbow Connector 37"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm rot="16200000" flipH="1">
-            <a:off x="401836" y="14963179"/>
-            <a:ext cx="2030015" cy="1095375"/>
+          <a:xfrm rot="5400000">
+            <a:off x="2103610" y="14998694"/>
+            <a:ext cx="1208895" cy="285748"/>
           </a:xfrm>
           <a:prstGeom prst="bentConnector3">
             <a:avLst>
@@ -352,203 +358,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="44" name="Straight Arrow Connector 43"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="869156" y="14608969"/>
-            <a:ext cx="0" cy="267891"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>39290</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>178594</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>107156</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="51" name="Group 50"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2617693" y="13564790"/>
-          <a:ext cx="1673460" cy="1591866"/>
-          <a:chOff x="2618116" y="14326790"/>
-          <a:chExt cx="1338129" cy="1591866"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="32" name="Elbow Connector 31"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000" flipH="1">
-            <a:off x="2491248" y="14453658"/>
-            <a:ext cx="1591866" cy="1338129"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="47" name="Straight Arrow Connector 46"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3953444" y="15406687"/>
-            <a:ext cx="0" cy="410766"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666752</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>184547</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>125015</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="96" name="Group 95"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2560546" y="15424547"/>
-          <a:ext cx="478348" cy="321468"/>
-          <a:chOff x="2562066" y="16186547"/>
-          <a:chExt cx="482906" cy="321468"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="38" name="Elbow Connector 37"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="5400000">
-            <a:off x="2642785" y="16105828"/>
-            <a:ext cx="321468" cy="482906"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 50000"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
           <xdr:cNvPr id="50" name="Straight Arrow Connector 49"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="3044972" y="16246078"/>
-            <a:ext cx="0" cy="113109"/>
+            <a:off x="2850931" y="14655885"/>
+            <a:ext cx="0" cy="425352"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -579,13 +395,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1023784</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -595,7 +411,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2917578" y="17354551"/>
+          <a:off x="2917578" y="16021051"/>
           <a:ext cx="190373" cy="523875"/>
           <a:chOff x="2918758" y="18116551"/>
           <a:chExt cx="183885" cy="523875"/>
@@ -673,13 +489,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1457325</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -689,7 +505,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1457325" y="16049625"/>
+          <a:off x="1457325" y="14716125"/>
           <a:ext cx="626969" cy="1771650"/>
           <a:chOff x="1457325" y="16811625"/>
           <a:chExt cx="628149" cy="1771650"/>
@@ -767,13 +583,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -783,7 +599,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2751044" y="16049625"/>
+          <a:off x="2751044" y="14716125"/>
           <a:ext cx="0" cy="1057275"/>
           <a:chOff x="2752224" y="16811625"/>
           <a:chExt cx="0" cy="1057275"/>
@@ -861,13 +677,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1051892</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>66261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1225826</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -877,7 +693,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2945686" y="16068261"/>
+          <a:off x="2945686" y="14734761"/>
           <a:ext cx="3658964" cy="422413"/>
           <a:chOff x="2948609" y="16830261"/>
           <a:chExt cx="3602934" cy="422413"/>
@@ -956,204 +772,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>364435</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>49697</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="76" name="Group 75"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="364435" y="19099697"/>
-          <a:ext cx="1600796" cy="2178325"/>
-          <a:chOff x="869156" y="14495859"/>
-          <a:chExt cx="1095375" cy="2030015"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="77" name="Elbow Connector 76"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000" flipH="1">
-            <a:off x="401836" y="14963179"/>
-            <a:ext cx="2030015" cy="1095375"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 50000"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="78" name="Straight Arrow Connector 77"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="869156" y="14608969"/>
-            <a:ext cx="0" cy="267891"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1496229</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>106525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>436054</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>75518</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="79" name="Group 78"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1496229" y="19156525"/>
-          <a:ext cx="1943001" cy="1492993"/>
-          <a:chOff x="2618116" y="14326790"/>
-          <a:chExt cx="1338129" cy="1591866"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="80" name="Elbow Connector 79"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="16200000" flipH="1">
-            <a:off x="2491248" y="14453658"/>
-            <a:ext cx="1591866" cy="1338129"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="81" name="Straight Arrow Connector 80"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3953444" y="15406687"/>
-            <a:ext cx="0" cy="410766"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>1807765</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>4397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>147272</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1163,7 +789,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1807765" y="22864397"/>
+          <a:off x="1807765" y="20006897"/>
           <a:ext cx="190804" cy="523875"/>
           <a:chOff x="2918758" y="18116551"/>
           <a:chExt cx="183885" cy="523875"/>
@@ -1241,13 +867,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1340094</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>25645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>73269</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>82795</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1257,7 +883,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1340094" y="21552145"/>
+          <a:off x="1340094" y="18694645"/>
           <a:ext cx="626969" cy="1771650"/>
           <a:chOff x="1457325" y="16811625"/>
           <a:chExt cx="628149" cy="1771650"/>
@@ -1335,13 +961,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>534865</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>25644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>534865</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>130419</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1351,7 +977,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2428659" y="21552144"/>
+          <a:off x="2428659" y="18694644"/>
           <a:ext cx="0" cy="1057275"/>
           <a:chOff x="2752224" y="16811625"/>
           <a:chExt cx="0" cy="1057275"/>
@@ -1429,13 +1055,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>963969</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>51607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1137903</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>93020</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1445,7 +1071,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2857763" y="21578107"/>
+          <a:off x="2857763" y="18720607"/>
           <a:ext cx="3658964" cy="422413"/>
           <a:chOff x="2948609" y="16830261"/>
           <a:chExt cx="3602934" cy="422413"/>
@@ -1524,43 +1150,41 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>791308</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
+      <xdr:colOff>347381</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>56027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>160274</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>138295</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>537879</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>156880</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="97" name="Group 96"/>
+        <xdr:cNvPr id="46" name="Group 45"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="2685102" y="20962327"/>
-          <a:ext cx="478348" cy="321468"/>
-          <a:chOff x="2562066" y="16186547"/>
-          <a:chExt cx="482906" cy="321468"/>
+        <a:xfrm rot="10800000">
+          <a:off x="2241175" y="17772527"/>
+          <a:ext cx="190498" cy="672353"/>
+          <a:chOff x="2752224" y="16811625"/>
+          <a:chExt cx="0" cy="1057275"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="98" name="Elbow Connector 97"/>
+          <xdr:cNvPr id="48" name="Straight Arrow Connector 47"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm rot="5400000">
-            <a:off x="2642785" y="16105828"/>
-            <a:ext cx="321468" cy="482906"/>
+          <a:xfrm>
+            <a:off x="2752224" y="16811625"/>
+            <a:ext cx="0" cy="1057275"/>
           </a:xfrm>
-          <a:prstGeom prst="bentConnector3">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 50000"/>
-            </a:avLst>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
           </a:prstGeom>
           <a:ln>
             <a:headEnd type="triangle"/>
@@ -1584,13 +1208,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="99" name="Straight Arrow Connector 98"/>
+          <xdr:cNvPr id="49" name="Straight Arrow Connector 48"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="3044972" y="16246078"/>
-            <a:ext cx="0" cy="113109"/>
+          <a:xfrm>
+            <a:off x="2752224" y="17551065"/>
+            <a:ext cx="0" cy="215566"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -1909,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,12 +1554,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1960,510 +1584,516 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
+      <c r="A13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
+      <c r="A17" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>10</v>
+      <c r="A20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>44</v>
+      <c r="G27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>18</v>
       </c>
-      <c r="C30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="E32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="I47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="I48" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" t="s">
-        <v>37</v>
-      </c>
-      <c r="I46" t="s">
-        <v>40</v>
-      </c>
-      <c r="K46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>21</v>
       </c>
-      <c r="G50" t="s">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>22</v>
       </c>
-      <c r="I50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" t="s">
-        <v>24</v>
-      </c>
-      <c r="K51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="I52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I54" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I55" t="s">
-        <v>27</v>
-      </c>
+      <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K56" s="1"/>
+      <c r="A56" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>46</v>
-      </c>
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+      <c r="A62" s="2"/>
       <c r="C62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="I62" s="1"/>
+      <c r="I62" s="4"/>
       <c r="K62" s="1"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="I63" s="4"/>
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="K64" s="1"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C69" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F80" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C81" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J81" s="7" t="s">
-        <v>27</v>
+      <c r="H80" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I80" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>2</v>
+      <c r="C84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F86" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F87" s="6" t="s">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G87" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I87" s="7" t="s">
+      <c r="B88" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>41</v>
+      <c r="C88" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A91" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>38</v>
-      </c>
-      <c r="K94" s="1"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="A98" s="5"/>
+      <c r="B98" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
@@ -2471,8 +2101,12 @@
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
+      <c r="F101" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
@@ -2482,6 +2116,10 @@
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
@@ -2491,6 +2129,10 @@
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
@@ -2507,7 +2149,9 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
+      <c r="B105" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
@@ -2558,7 +2202,9 @@
       <c r="K108" s="5"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
+      <c r="A109" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -2573,9 +2219,7 @@
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="5"/>
-      <c r="C110" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
@@ -2599,215 +2243,94 @@
       <c r="K111" s="5"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
       <c r="K112" s="5"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
+    <row r="113" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
       <c r="K113" s="5"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="5"/>
-      <c r="I114" s="5"/>
+    <row r="114" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J114" s="5"/>
       <c r="K114" s="5"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="5"/>
-      <c r="I115" s="5"/>
+    <row r="115" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J115" s="5"/>
       <c r="K115" s="5"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G116" s="5"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="5"/>
+    <row r="116" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J116" s="5"/>
       <c r="K116" s="5"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
+    <row r="117" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J117" s="5"/>
       <c r="K117" s="5"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="5"/>
+    <row r="118" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J118" s="5"/>
       <c r="K118" s="5"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="5"/>
-      <c r="K119" s="5"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="5"/>
-      <c r="B120" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
+    <row r="120" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G120" s="5"/>
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
       <c r="K120" s="5"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
+    <row r="121" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
       <c r="K121" s="5"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
+    <row r="122" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G122" s="5"/>
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
       <c r="K122" s="5"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
+    <row r="123" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
       <c r="K123" s="5"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B124" s="5"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
+    <row r="124" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
       <c r="K124" s="5"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
+    <row r="125" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
       <c r="J125" s="5"/>
       <c r="K125" s="5"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="5"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
+    <row r="126" spans="7:11" x14ac:dyDescent="0.25">
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
       <c r="J126" s="5"/>
       <c r="K126" s="5"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:11" x14ac:dyDescent="0.25">
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
       <c r="K127" s="5"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:11" x14ac:dyDescent="0.25">
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
@@ -2820,6 +2343,13 @@
       <c r="K129" s="5"/>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
@@ -2851,21 +2381,8 @@
       <c r="J132" s="5"/>
       <c r="K132" s="5"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
-      <c r="H133" s="5"/>
-      <c r="I133" s="5"/>
-      <c r="J133" s="5"/>
-      <c r="K133" s="5"/>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="3"/>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>

</xml_diff>

<commit_message>
Updatet db docs, revisies, intergrale systeemtest, bug fixes en comments
</commit_message>
<xml_diff>
--- a/Documentatie/KT2/ad.2.1_Genormaliseerde_databaseontwerp.xlsx
+++ b/Documentatie/KT2/ad.2.1_Genormaliseerde_databaseontwerp.xlsx
@@ -61,9 +61,6 @@
     <t>SubjectName</t>
   </si>
   <si>
-    <t>AppointmentDescription</t>
-  </si>
-  <si>
     <t>TaskDate</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>•SubjectName</t>
   </si>
   <si>
-    <t>•AppointmentDescription</t>
-  </si>
-  <si>
     <t>•TaskTitle</t>
   </si>
   <si>
@@ -221,6 +215,12 @@
   </si>
   <si>
     <t>Grades</t>
+  </si>
+  <si>
+    <t>•AppointmentName</t>
+  </si>
+  <si>
+    <t>AppointmentName</t>
   </si>
 </sst>
 </file>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1576,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1591,17 +1591,17 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1611,72 +1611,72 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1719,19 +1719,19 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" t="s">
         <v>64</v>
-      </c>
-      <c r="G34" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1742,13 +1742,13 @@
         <v>4</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>5</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
@@ -1776,39 +1776,39 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
       </c>
       <c r="I38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K38" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="I39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K39" t="s">
         <v>9</v>
@@ -1816,31 +1816,31 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1864,45 +1864,45 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F57" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -1913,16 +1913,16 @@
         <v>0</v>
       </c>
       <c r="G60" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H60" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="7" t="s">
+      <c r="J60" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -1946,7 +1946,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J67" s="7" t="s">
         <v>9</v>
@@ -1965,34 +1965,34 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D76" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>0</v>
       </c>
       <c r="F76" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H76" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>0</v>
@@ -2006,16 +2006,16 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
@@ -2055,7 +2055,7 @@
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
       <c r="C91" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -2085,7 +2085,7 @@
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2114,10 +2114,10 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>

</xml_diff>